<commit_message>
[FIX] UAT Budget Unit Base
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="budget_breakdown" sheetId="1" state="visible" r:id="rId2"/>
@@ -89,11 +89,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,18 +157,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FFFF3333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -232,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,7 +230,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,6 +246,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,11 +258,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,11 +270,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,15 +278,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,120 +369,114 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="I:J"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.219387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="24.219387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7602040816327"/>
-    <col collapsed="false" hidden="true" max="10" min="9" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="19.9081632653061"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.76"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="19.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="7" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
+      <c r="B3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="s">
+      <c r="B4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="11"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
+      <c r="B6" s="13"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
+      <c r="B7" s="13"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="13" t="n">
         <f aca="false">SUM(G12:G5000)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="13" t="n">
         <f aca="false">B8-B7</f>
         <v>0</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -499,16 +486,16 @@
       <c r="C11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="0" t="s">
@@ -521,7 +508,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[ENH] fix budget breakdown excel sheet
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Budget Breakdown</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rolling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release</t>
   </si>
   <si>
     <t xml:space="preserve">Latest Policy Amount</t>
@@ -367,23 +370,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.76"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.76"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="19.91"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,6 +400,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8"/>
@@ -406,7 +411,8 @@
       <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
@@ -417,7 +423,8 @@
       <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
@@ -428,40 +435,41 @@
       <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="13" t="n">
-        <f aca="false">SUM(G12:G5000)</f>
+        <f aca="false">SUM(H12:H5000)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -469,14 +477,14 @@
         <f aca="false">B8-B7</f>
         <v>0</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="12" t="s">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -496,13 +504,16 @@
         <v>18</v>
       </c>
       <c r="G11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>10</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ENH] pabi_budget_plan, add check column in breakdown
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_breakdown_unit_base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Budget Breakdown</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Latest Policy Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check</t>
   </si>
   <si>
     <t xml:space="preserve">budget_id</t>
@@ -224,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +244,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,6 +258,10 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -291,6 +302,10 @@
     </xf>
     <xf numFmtId="166" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -385,135 +400,139 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="13.76"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="19.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="9" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="0"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="10" t="s">
+      <c r="B3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="10" t="s">
+      <c r="B4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="13" t="n">
+      <c r="B8" s="15" t="n">
         <f aca="false">SUM(H12:H5000)</f>
         <v>0</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13" t="n">
+      <c r="B9" s="15" t="n">
         <f aca="false">B8-B7</f>
         <v>0</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="18" t="s">
         <v>10</v>
       </c>
+      <c r="I11" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="J11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>